<commit_message>
Added better graphs with all 3 metabolites on them
</commit_message>
<xml_diff>
--- a/AIC7parameters_hptoolbox_moredata.xlsx
+++ b/AIC7parameters_hptoolbox_moredata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA56BF9-F290-4910-B067-2032C05AA27B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05135A9-05DD-490F-83B9-18A8186E72E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="13932" windowWidth="21600" windowHeight="11388" xr2:uid="{7B797320-3572-489B-A3DE-9B4D4211A2D6}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11325" xr2:uid="{7B797320-3572-489B-A3DE-9B4D4211A2D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -596,13 +596,13 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2627.8266118027918</v>
+        <v>2576.2845482917992</v>
       </c>
       <c r="B20">
-        <v>2012.888568557466</v>
+        <v>1981.3402408926472</v>
       </c>
       <c r="C20">
-        <v>1908.2749824878156</v>
+        <v>1870.1560410687173</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ran AIC comparison with klp and kinflux set to 0
</commit_message>
<xml_diff>
--- a/AIC7parameters_hptoolbox_moredata.xlsx
+++ b/AIC7parameters_hptoolbox_moredata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FECDEF1-4F6B-4EE3-88D9-47310F27DF61}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9716F245-370C-4AC6-B3A0-B09B047199B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11325" xr2:uid="{7B797320-3572-489B-A3DE-9B4D4211A2D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7B797320-3572-489B-A3DE-9B4D4211A2D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -377,15 +377,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F274502-9980-4688-A2D5-4743D4450742}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C22"/>
+      <selection activeCell="F1" sqref="F1:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2504.3641875225248</v>
       </c>
@@ -395,8 +395,20 @@
       <c r="C1">
         <v>1659.175700557744</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F1">
+        <f>A1-2*10+2*9</f>
+        <v>2502.3641875225248</v>
+      </c>
+      <c r="G1">
+        <f t="shared" ref="G1:H16" si="0">B1-2*10+2*9</f>
+        <v>1673.4817733253944</v>
+      </c>
+      <c r="H1">
+        <f t="shared" si="0"/>
+        <v>1657.175700557744</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2262.5551341635014</v>
       </c>
@@ -406,8 +418,20 @@
       <c r="C2">
         <v>1376.2941818763427</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f t="shared" ref="F2:F22" si="1">A2-2*10+2*9</f>
+        <v>2260.5551341635014</v>
+      </c>
+      <c r="G2">
+        <f t="shared" si="0"/>
+        <v>1500.7606434992442</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>1374.2941818763427</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2560.3680356691543</v>
       </c>
@@ -417,8 +441,20 @@
       <c r="C3">
         <v>1579.0404426421503</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <f t="shared" si="1"/>
+        <v>2558.3680356691543</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>1738.6138750621997</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>1577.0404426421503</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2494.2816724362074</v>
       </c>
@@ -428,8 +464,20 @@
       <c r="C4">
         <v>1890.1705214780602</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>2492.2816724362074</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>1884.0880077709817</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>1888.1705214780602</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2528.8038651354173</v>
       </c>
@@ -439,8 +487,20 @@
       <c r="C5">
         <v>1754.8834586714404</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>2526.8038651354173</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>1750.8912484338457</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>1752.8834586714404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2478.7488923483206</v>
       </c>
@@ -450,8 +510,20 @@
       <c r="C6">
         <v>1881.3871662939919</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>2476.7488923483206</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>1824.3368947729757</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1879.3871662939919</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2397.2088800618067</v>
       </c>
@@ -461,8 +533,20 @@
       <c r="C7">
         <v>1675.6638407780397</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>2395.2088800618067</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>1846.4308520432855</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>1673.6638407780397</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2467.996998375711</v>
       </c>
@@ -472,8 +556,20 @@
       <c r="C8">
         <v>1785.2198927447378</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>2465.996998375711</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1928.0307207430074</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>1783.2198927447378</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2643.8788680913858</v>
       </c>
@@ -483,8 +579,20 @@
       <c r="C9">
         <v>1635.4856174790666</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>2641.8788680913858</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>1941.4610312448535</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>1633.4856174790666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2394.9108173457316</v>
       </c>
@@ -494,8 +602,20 @@
       <c r="C10">
         <v>1429.4701744687366</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>2392.9108173457316</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1518.2078910823648</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>1427.4701744687366</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2163.0433237002462</v>
       </c>
@@ -505,8 +625,20 @@
       <c r="C11">
         <v>1407.2570777772714</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>2161.0433237002462</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>1573.4311100229684</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>1405.2570777772714</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2770.6264484910107</v>
       </c>
@@ -516,8 +648,20 @@
       <c r="C12">
         <v>1875.0922041911349</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>2768.6264484910107</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>2191.8789571331267</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>1873.0922041911349</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2528.1018186655519</v>
       </c>
@@ -527,8 +671,20 @@
       <c r="C13">
         <v>1754.633454248107</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>2526.1018186655519</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>1946.3587415276781</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>1752.633454248107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2609.7077573736137</v>
       </c>
@@ -538,8 +694,20 @@
       <c r="C14">
         <v>1759.3304433006706</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>2607.7077573736137</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>2016.5644302498422</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>1757.3304433006706</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2498.8845153969119</v>
       </c>
@@ -549,8 +717,20 @@
       <c r="C15">
         <v>1838.8582161258253</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>2496.8845153969119</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>2024.4017199517746</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>1836.8582161258253</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2592.3756000667886</v>
       </c>
@@ -560,8 +740,20 @@
       <c r="C16">
         <v>1554.7405201260492</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>2590.3756000667886</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>1794.2617606532046</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>1552.7405201260492</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2355.9502413785494</v>
       </c>
@@ -571,8 +763,20 @@
       <c r="C17">
         <v>1699.7042402819582</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>2353.9502413785494</v>
+      </c>
+      <c r="G17">
+        <f t="shared" ref="G17:G22" si="2">B17-2*10+2*9</f>
+        <v>1783.7963220480617</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ref="H17:H22" si="3">C17-2*10+2*9</f>
+        <v>1697.7042402819582</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2615.6965196820511</v>
       </c>
@@ -582,8 +786,20 @@
       <c r="C18">
         <v>2083.448066940392</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>2613.6965196820511</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>2160.0331228077912</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="3"/>
+        <v>2081.448066940392</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2011.2296828283734</v>
       </c>
@@ -593,8 +809,20 @@
       <c r="C19">
         <v>1981.0689856943163</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>2009.2296828283734</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>2031.9312076960384</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="3"/>
+        <v>1979.0689856943163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2576.2845482917992</v>
       </c>
@@ -604,8 +832,20 @@
       <c r="C20">
         <v>1870.1560410687173</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>2574.2845482917992</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>1979.3402408926472</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="3"/>
+        <v>1868.1560410687173</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2713.0802000001959</v>
       </c>
@@ -615,8 +855,20 @@
       <c r="C21">
         <v>1980.6742389564292</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>2711.0802000001959</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>2018.8570413855018</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="3"/>
+        <v>1978.6742389564292</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2569.5114382281931</v>
       </c>
@@ -625,6 +877,18 @@
       </c>
       <c r="C22">
         <v>1732.1200200450439</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>2567.5114382281931</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>1980.4267725062407</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="3"/>
+        <v>1730.1200200450439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
These are the images with 7 param model
</commit_message>
<xml_diff>
--- a/AIC7parameters_hptoolbox_moredata.xlsx
+++ b/AIC7parameters_hptoolbox_moredata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9716F245-370C-4AC6-B3A0-B09B047199B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D24229C-ECB7-41C1-AC96-094604432B27}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7B797320-3572-489B-A3DE-9B4D4211A2D6}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{7B797320-3572-489B-A3DE-9B4D4211A2D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -377,518 +377,529 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F274502-9980-4688-A2D5-4743D4450742}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H22"/>
+      <selection sqref="A1:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2504.3641875225248</v>
+        <v>2504.3641872458752</v>
       </c>
       <c r="B1">
-        <v>1675.4817733253944</v>
+        <v>1680.6863481769783</v>
       </c>
       <c r="C1">
-        <v>1659.175700557744</v>
+        <v>1660.8938869597118</v>
       </c>
       <c r="F1">
         <f>A1-2*10+2*9</f>
-        <v>2502.3641875225248</v>
+        <v>2502.3641872458752</v>
       </c>
       <c r="G1">
         <f t="shared" ref="G1:H16" si="0">B1-2*10+2*9</f>
-        <v>1673.4817733253944</v>
+        <v>1678.6863481769783</v>
       </c>
       <c r="H1">
         <f t="shared" si="0"/>
-        <v>1657.175700557744</v>
+        <v>1658.8938869597118</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2262.5551341635014</v>
+        <v>2262.55694124916</v>
       </c>
       <c r="B2">
-        <v>1502.7606434992442</v>
+        <v>1504.6477254743138</v>
       </c>
       <c r="C2">
-        <v>1376.2941818763427</v>
+        <v>1375.3170900420705</v>
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F22" si="1">A2-2*10+2*9</f>
-        <v>2260.5551341635014</v>
+        <v>2260.55694124916</v>
       </c>
       <c r="G2">
         <f t="shared" si="0"/>
-        <v>1500.7606434992442</v>
+        <v>1502.6477254743138</v>
       </c>
       <c r="H2">
         <f t="shared" si="0"/>
-        <v>1374.2941818763427</v>
+        <v>1373.3170900420705</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2560.3680356691543</v>
+        <v>2560.3680528721502</v>
       </c>
       <c r="B3">
-        <v>1740.6138750621997</v>
+        <v>1740.2667114603717</v>
       </c>
       <c r="C3">
-        <v>1579.0404426421503</v>
+        <v>1585.0832652976844</v>
       </c>
       <c r="F3">
         <f t="shared" si="1"/>
-        <v>2558.3680356691543</v>
+        <v>2558.3680528721502</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
-        <v>1738.6138750621997</v>
+        <v>1738.2667114603717</v>
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
-        <v>1577.0404426421503</v>
+        <v>1583.0832652976844</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2494.2816724362074</v>
+        <v>2494.2847112728741</v>
       </c>
       <c r="B4">
-        <v>1886.0880077709817</v>
+        <v>1887.6398329156857</v>
       </c>
       <c r="C4">
-        <v>1890.1705214780602</v>
+        <v>1890.9331066616555</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>2492.2816724362074</v>
+        <v>2492.2847112728741</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>1884.0880077709817</v>
+        <v>1885.6398329156857</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>1888.1705214780602</v>
+        <v>1888.9331066616555</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2528.8038651354173</v>
+        <v>2528.8038454788189</v>
       </c>
       <c r="B5">
-        <v>1752.8912484338457</v>
+        <v>1753.003727639835</v>
       </c>
       <c r="C5">
-        <v>1754.8834586714404</v>
+        <v>1754.5421504869457</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>2526.8038651354173</v>
+        <v>2526.8038454788189</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>1750.8912484338457</v>
+        <v>1751.003727639835</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>1752.8834586714404</v>
+        <v>1752.5421504869457</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2478.7488923483206</v>
+        <v>2478.7459565060203</v>
       </c>
       <c r="B6">
-        <v>1826.3368947729757</v>
+        <v>1828.9944935750555</v>
       </c>
       <c r="C6">
-        <v>1881.3871662939919</v>
+        <v>1882.8313575376681</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>2476.7488923483206</v>
+        <v>2476.7459565060203</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>1824.3368947729757</v>
+        <v>1826.9944935750555</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>1879.3871662939919</v>
+        <v>1880.8313575376681</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2397.2088800618067</v>
+        <v>2397.2095768963327</v>
       </c>
       <c r="B7">
-        <v>1848.4308520432855</v>
+        <v>1849.4812563282758</v>
       </c>
       <c r="C7">
-        <v>1675.6638407780397</v>
+        <v>1679.6191375567414</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>2395.2088800618067</v>
+        <v>2395.2095768963327</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>1846.4308520432855</v>
+        <v>1847.4812563282758</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>1673.6638407780397</v>
+        <v>1677.6191375567414</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2467.996998375711</v>
+        <v>2467.9970013459274</v>
       </c>
       <c r="B8">
-        <v>1930.0307207430074</v>
+        <v>1930.0372423531173</v>
       </c>
       <c r="C8">
-        <v>1785.2198927447378</v>
+        <v>1785.1941432769693</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>2465.996998375711</v>
+        <v>2465.9970013459274</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>1928.0307207430074</v>
+        <v>1928.0372423531173</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>1783.2198927447378</v>
+        <v>1783.1941432769693</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2643.8788680913858</v>
+        <v>2643.8788154272052</v>
       </c>
       <c r="B9">
-        <v>1943.4610312448535</v>
+        <v>1943.475416109985</v>
       </c>
       <c r="C9">
-        <v>1635.4856174790666</v>
+        <v>1635.4938427291459</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>2641.8788680913858</v>
+        <v>2641.8788154272052</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>1941.4610312448535</v>
+        <v>1941.475416109985</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>1633.4856174790666</v>
+        <v>1633.4938427291459</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2394.9108173457316</v>
+        <v>2394.9100913362677</v>
       </c>
       <c r="B10">
-        <v>1520.2078910823648</v>
+        <v>1530.383635317052</v>
       </c>
       <c r="C10">
-        <v>1429.4701744687366</v>
+        <v>1428.9671136278478</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>2392.9108173457316</v>
+        <v>2392.9100913362677</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>1518.2078910823648</v>
+        <v>1528.383635317052</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>1427.4701744687366</v>
+        <v>1426.9671136278478</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2163.0433237002462</v>
+        <v>2163.0424132805206</v>
       </c>
       <c r="B11">
-        <v>1575.4311100229684</v>
+        <v>1575.4338612267611</v>
       </c>
       <c r="C11">
-        <v>1407.2570777772714</v>
+        <v>1407.2526586545646</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>2161.0433237002462</v>
+        <v>2161.0424132805206</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>1573.4311100229684</v>
+        <v>1573.4338612267611</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>1405.2570777772714</v>
+        <v>1405.2526586545646</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2770.6264484910107</v>
+        <v>2770.6264489143277</v>
       </c>
       <c r="B12">
-        <v>2193.8789571331267</v>
+        <v>2193.8783156302029</v>
       </c>
       <c r="C12">
-        <v>1875.0922041911349</v>
+        <v>1875.1465558948457</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>2768.6264484910107</v>
+        <v>2768.6264489143277</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>2191.8789571331267</v>
+        <v>2191.8783156302029</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>1873.0922041911349</v>
+        <v>1873.1465558948457</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2528.1018186655519</v>
+        <v>2528.0865774114127</v>
       </c>
       <c r="B13">
-        <v>1948.3587415276781</v>
+        <v>1958.223367122167</v>
       </c>
       <c r="C13">
-        <v>1754.633454248107</v>
+        <v>1765.5967950965151</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>2526.1018186655519</v>
+        <v>2526.0865774114127</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>1946.3587415276781</v>
+        <v>1956.223367122167</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>1752.633454248107</v>
+        <v>1763.5967950965151</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2609.7077573736137</v>
+        <v>2609.7137253488277</v>
       </c>
       <c r="B14">
-        <v>2018.5644302498422</v>
+        <v>2022.9225150705993</v>
       </c>
       <c r="C14">
-        <v>1759.3304433006706</v>
+        <v>1756.5472354606577</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>2607.7077573736137</v>
+        <v>2607.7137253488277</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>2016.5644302498422</v>
+        <v>2020.9225150705993</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>1757.3304433006706</v>
+        <v>1754.5472354606577</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2498.8845153969119</v>
+        <v>2498.9596433937973</v>
       </c>
       <c r="B15">
-        <v>2026.4017199517746</v>
+        <v>2031.0777341711305</v>
       </c>
       <c r="C15">
-        <v>1838.8582161258253</v>
+        <v>1838.001306978955</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>2496.8845153969119</v>
+        <v>2496.9596433937973</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>2024.4017199517746</v>
+        <v>2029.0777341711305</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>1836.8582161258253</v>
+        <v>1836.001306978955</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2592.3756000667886</v>
+        <v>2592.3756656780934</v>
       </c>
       <c r="B16">
-        <v>1796.2617606532046</v>
+        <v>1796.2257130653136</v>
       </c>
       <c r="C16">
-        <v>1554.7405201260492</v>
+        <v>1555.3439003568135</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>2590.3756000667886</v>
+        <v>2590.3756656780934</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>1794.2617606532046</v>
+        <v>1794.2257130653136</v>
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>1552.7405201260492</v>
+        <v>1553.3439003568135</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2355.9502413785494</v>
+        <v>2355.9379710138674</v>
       </c>
       <c r="B17">
-        <v>1785.7963220480617</v>
+        <v>1789.6481733224953</v>
       </c>
       <c r="C17">
-        <v>1699.7042402819582</v>
+        <v>1700.6493438790021</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>2353.9502413785494</v>
+        <v>2353.9379710138674</v>
       </c>
       <c r="G17">
         <f t="shared" ref="G17:G22" si="2">B17-2*10+2*9</f>
-        <v>1783.7963220480617</v>
+        <v>1787.6481733224953</v>
       </c>
       <c r="H17">
         <f t="shared" ref="H17:H22" si="3">C17-2*10+2*9</f>
-        <v>1697.7042402819582</v>
+        <v>1698.6493438790021</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2615.6965196820511</v>
+        <v>2615.4880450976702</v>
       </c>
       <c r="B18">
-        <v>2162.0331228077912</v>
+        <v>2163.4214778065211</v>
       </c>
       <c r="C18">
-        <v>2083.448066940392</v>
+        <v>2077.8516997418374</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>2613.6965196820511</v>
+        <v>2613.4880450976702</v>
       </c>
       <c r="G18">
         <f t="shared" si="2"/>
-        <v>2160.0331228077912</v>
+        <v>2161.4214778065211</v>
       </c>
       <c r="H18">
         <f t="shared" si="3"/>
-        <v>2081.448066940392</v>
+        <v>2075.8516997418374</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2011.2296828283734</v>
+        <v>2011.2299318360142</v>
       </c>
       <c r="B19">
-        <v>2033.9312076960384</v>
+        <v>2033.9311347760126</v>
       </c>
       <c r="C19">
-        <v>1981.0689856943163</v>
+        <v>1981.0688096723513</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>2009.2296828283734</v>
+        <v>2009.2299318360142</v>
       </c>
       <c r="G19">
         <f t="shared" si="2"/>
-        <v>2031.9312076960384</v>
+        <v>2031.9311347760126</v>
       </c>
       <c r="H19">
         <f t="shared" si="3"/>
-        <v>1979.0689856943163</v>
+        <v>1979.0688096723513</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2576.2845482917992</v>
+        <v>2576.2750779554822</v>
       </c>
       <c r="B20">
-        <v>1981.3402408926472</v>
+        <v>1984.8956900048479</v>
       </c>
       <c r="C20">
-        <v>1870.1560410687173</v>
+        <v>1877.125556341239</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>2574.2845482917992</v>
+        <v>2574.2750779554822</v>
       </c>
       <c r="G20">
         <f t="shared" si="2"/>
-        <v>1979.3402408926472</v>
+        <v>1982.8956900048479</v>
       </c>
       <c r="H20">
         <f t="shared" si="3"/>
-        <v>1868.1560410687173</v>
+        <v>1875.125556341239</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2713.0802000001959</v>
+        <v>2713.0795141164522</v>
       </c>
       <c r="B21">
-        <v>2020.8570413855018</v>
+        <v>2022.0638328393798</v>
       </c>
       <c r="C21">
-        <v>1980.6742389564292</v>
+        <v>1981.0244367991929</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>2711.0802000001959</v>
+        <v>2711.0795141164522</v>
       </c>
       <c r="G21">
         <f t="shared" si="2"/>
-        <v>2018.8570413855018</v>
+        <v>2020.0638328393798</v>
       </c>
       <c r="H21">
         <f t="shared" si="3"/>
-        <v>1978.6742389564292</v>
+        <v>1979.0244367991929</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2569.5114382281931</v>
+        <v>2569.5114444116962</v>
       </c>
       <c r="B22">
-        <v>1982.4267725062407</v>
+        <v>1982.4537065438044</v>
       </c>
       <c r="C22">
-        <v>1732.1200200450439</v>
+        <v>1731.7631208362495</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>2567.5114382281931</v>
+        <v>2567.5114444116962</v>
       </c>
       <c r="G22">
         <f t="shared" si="2"/>
-        <v>1980.4267725062407</v>
+        <v>1980.4537065438044</v>
       </c>
       <c r="H22">
         <f t="shared" si="3"/>
-        <v>1730.1200200450439</v>
+        <v>1729.7631208362495</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2527.0568162501113</v>
+      </c>
+      <c r="B23">
+        <v>1686.8929203187608</v>
+      </c>
+      <c r="C23">
+        <v>1775.9525937170963</v>
       </c>
     </row>
   </sheetData>

</xml_diff>